<commit_message>
final updates for sending
</commit_message>
<xml_diff>
--- a/Envio correos/Correos personalizados Smart Forests 2 new.xlsx
+++ b/Envio correos/Correos personalizados Smart Forests 2 new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aa631587986ce8df/Documentos/VS Code/Python/Envio correos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{6E552543-A674-4774-A4BC-1490E40AB4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81C42904-D875-4F15-8E9D-88286244204F}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{6E552543-A674-4774-A4BC-1490E40AB4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E036773-3DE1-4C3A-A007-36A9F596C109}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2BC6CA2F-7348-4FAA-ABCC-A6ECB71E7F0C}"/>
   </bookViews>
@@ -45,13 +45,13 @@
     <t>Genero</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>Felipe</t>
   </si>
   <si>
     <t>felipe.guarda@fundacionmaradentro.cl</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -498,13 +498,13 @@
     </row>
     <row r="2" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>